<commit_message>
feat: change programme id value in plo excel
</commit_message>
<xml_diff>
--- a/public/template/plo-po.xlsx
+++ b/public/template/plo-po.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Desktop\CPE 402\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF276E29-3E8C-423D-9554-A2AF532B9606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8599A32-675D-42B6-AF13-52551EC24F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Year</t>
   </si>
@@ -59,9 +59,6 @@
     <t>สามารถ…</t>
   </si>
   <si>
-    <t>Able to…</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>Design…</t>
+  </si>
+  <si>
+    <t>Able to… (Optional)</t>
+  </si>
+  <si>
+    <t>ปีของหลักสูตร</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{217FCC4E-FA60-487B-91BF-8407B0889C38}" name="Table1" displayName="Table1" ref="A2:B3" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{217FCC4E-FA60-487B-91BF-8407B0889C38}" name="Table1" displayName="Table1" ref="A2:B3" totalsRowShown="0">
   <autoFilter ref="A2:B3" xr:uid="{217FCC4E-FA60-487B-91BF-8407B0889C38}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6486706C-88B2-4FEE-A990-EA3AD07886AD}" name="_Curriculum"/>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -470,6 +473,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
@@ -489,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -500,7 +508,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{644D5A9C-A6DB-474B-B803-91611F4F8D25}">
-      <formula1>"Thai,Inter"</formula1>
+      <formula1>"regular,inter"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -515,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46770CF-0A86-4130-9EA2-CFBA896C7198}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -528,15 +536,15 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -553,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +596,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -618,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
feat: update po-plo template
</commit_message>
<xml_diff>
--- a/public/template/plo-po.xlsx
+++ b/public/template/plo-po.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8599A32-675D-42B6-AF13-52551EC24F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC678DA7-6F88-4AB0-B02E-95F1C866F9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Year</t>
   </si>
@@ -77,10 +77,28 @@
     <t>Design…</t>
   </si>
   <si>
-    <t>Able to… (Optional)</t>
-  </si>
-  <si>
-    <t>ปีของหลักสูตร</t>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>2564 (พ.ศ.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to… </t>
+  </si>
+  <si>
+    <t>(Optional)</t>
+  </si>
+  <si>
+    <t>แปลว่า Sub PLO 1.2</t>
+  </si>
+  <si>
+    <t>* ถ้า import ด้วย template นี้ จะต้องใส่ Sub-PLO ไปพร้อมกับ PLO</t>
+  </si>
+  <si>
+    <t>* ไม่จำเป็นต้อง import ไปพร้อมกับ PLO, Sub-PLO</t>
   </si>
 </sst>
 </file>
@@ -446,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -460,25 +478,32 @@
     <col min="4" max="4" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -488,21 +513,22 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -521,10 +547,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46770CF-0A86-4130-9EA2-CFBA896C7198}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -534,12 +560,15 @@
     <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -552,35 +581,28 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -593,10 +615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A38076-9583-4F37-89F2-DC107EF02173}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -605,12 +627,15 @@
     <col min="3" max="3" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -620,21 +645,17 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>